<commit_message>
Update Work Plan Template v2.xlsx
</commit_message>
<xml_diff>
--- a/mypath/Work Plan Template v2.xlsx
+++ b/mypath/Work Plan Template v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tcrow\Documents\Src\Python\reddit\mypath\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA65967-6F99-4536-A50A-BD21F59D2A51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFE2FE5-69AA-4EDD-8096-BF2D7F535394}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3405" yWindow="2640" windowWidth="22530" windowHeight="12030" xr2:uid="{205A3DD4-7EB7-4A50-B1BD-A5C72ACE3C1D}"/>
   </bookViews>
@@ -408,9 +408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72B65DB5-0EB8-4D40-87FA-C8301E0B3902}">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>